<commit_message>
versão 2.0. bug ainda não corrigido
</commit_message>
<xml_diff>
--- a/casos_por_tipo.xlsx
+++ b/casos_por_tipo.xlsx
@@ -460,10 +460,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>4676</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>80.55</v>
       </c>
     </row>
     <row r="3">
@@ -476,10 +476,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>1066</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>18.36</v>
       </c>
     </row>
     <row r="4">
@@ -492,10 +492,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="5">
@@ -508,10 +508,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>5805</v>
+        <v>28</v>
       </c>
       <c r="D5" t="n">
-        <v>100</v>
+        <v>0.48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>